<commit_message>
Mise à dispo de tous les éléments IHM + dossier maquettage IHM
- rendus
- psd
- textures
- actu suivi charges
- maquettage IHM
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>TACHES</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Composition du classeur de projet</t>
+  </si>
+  <si>
+    <t>Rédaction du dossier maquettage Ihm</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="B2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,14 +695,26 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
@@ -792,7 +807,11 @@
       <c r="D42" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D22"/>
+  <autoFilter ref="B2:D22">
+    <sortState ref="B3:D24">
+      <sortCondition ref="C2:C22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à dispo de documents projet
- Maj du gantt sous Microsoft project
- Maj du suivi d’activités liechti
- Maj du tableau de suivi d’activités
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>TACHES</t>
   </si>
@@ -31,9 +31,6 @@
     <t>TEMPS (H)</t>
   </si>
   <si>
-    <t>Conception maquette IHM</t>
-  </si>
-  <si>
     <t>Rédaction compte rendu réunion 01</t>
   </si>
   <si>
@@ -68,6 +65,24 @@
   </si>
   <si>
     <t>Composition du classeur de projet</t>
+  </si>
+  <si>
+    <t>Rédaction du dossier maquettage Ihm</t>
+  </si>
+  <si>
+    <t>Conception maquette IHM photoshop</t>
+  </si>
+  <si>
+    <t>Installation d'un raspberry de test</t>
+  </si>
+  <si>
+    <t>Actualisation suivi d'activité</t>
+  </si>
+  <si>
+    <t>Actualisation du gantt</t>
+  </si>
+  <si>
+    <t>Actualisation suivi des tâches</t>
   </si>
 </sst>
 </file>
@@ -449,7 +464,7 @@
   <dimension ref="B2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +488,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3">
         <v>42255</v>
@@ -484,7 +499,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>42259</v>
@@ -495,7 +510,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>42260</v>
@@ -506,7 +521,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>42261</v>
@@ -517,7 +532,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>42263</v>
@@ -528,7 +543,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3">
         <v>42264</v>
@@ -539,7 +554,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
         <v>42268</v>
@@ -550,7 +565,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3">
         <v>42270</v>
@@ -561,7 +576,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>42272</v>
@@ -572,7 +587,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>42275</v>
@@ -583,7 +598,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
         <v>42275</v>
@@ -594,7 +609,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
         <v>42279</v>
@@ -605,7 +620,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3">
         <v>42284</v>
@@ -616,7 +631,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3">
         <v>42287</v>
@@ -627,7 +642,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3">
         <v>42289</v>
@@ -638,7 +653,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3">
         <v>42291</v>
@@ -649,7 +664,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3">
         <v>42311</v>
@@ -660,7 +675,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C20" s="3">
         <v>42315</v>
@@ -671,7 +686,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3">
         <v>42316</v>
@@ -682,7 +697,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C22" s="3">
         <v>42318</v>
@@ -692,34 +707,70 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42326</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42326</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3">
+        <v>42326</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3">
+        <v>42326</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
@@ -792,7 +843,11 @@
       <c r="D42" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D22"/>
+  <autoFilter ref="B2:D22">
+    <sortState ref="B3:D24">
+      <sortCondition ref="C2:C22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Maj docs suivi de projet
- suivi perso
- suivi taches
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
@@ -16,12 +16,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$K$39</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>TACHES</t>
   </si>
@@ -90,6 +89,15 @@
   </si>
   <si>
     <t>Construction de la base de données SQL sur le raspberry</t>
+  </si>
+  <si>
+    <t>Travail sur les textures photoshop</t>
+  </si>
+  <si>
+    <t>Reprise fichiers templates pour responsive design</t>
+  </si>
+  <si>
+    <t>Modification organisation arborsence application</t>
   </si>
 </sst>
 </file>
@@ -471,7 +479,7 @@
   <dimension ref="B2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,24 +810,48 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="3">
+        <v>42329</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42331</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="3">
+        <v>42336</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="3">
+        <v>42336</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>

</xml_diff>

<commit_message>
Maj gestion de projet
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_liechti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="5820" yWindow="570" windowWidth="14280" windowHeight="12750"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$D$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$D$69</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$K$38</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>TACHES</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>TEMPS TOTAL (H)</t>
+  </si>
+  <si>
+    <t>Construction des pages</t>
+  </si>
+  <si>
+    <t>Scripting shell sur Raspberry</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F68"/>
+  <dimension ref="B2:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +530,7 @@
       </c>
       <c r="F3" s="5">
         <f>SUM(D3:D90)</f>
-        <v>95.7</v>
+        <v>152.19999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1012,113 +1018,355 @@
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3">
+        <v>42348</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="B49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="3">
+        <v>42353</v>
+      </c>
+      <c r="D49" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="B50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="3">
+        <v>42354</v>
+      </c>
+      <c r="D50" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="3">
+        <v>42364</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="3">
+        <v>42364</v>
+      </c>
+      <c r="D52" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="3">
+        <v>42364</v>
+      </c>
+      <c r="D53" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="3">
+        <v>42365</v>
+      </c>
+      <c r="D54" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="B55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="3">
+        <v>42367</v>
+      </c>
+      <c r="D55" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="3">
+        <v>42367</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="3">
+        <v>42367</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="B58" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="3">
+        <v>42371</v>
+      </c>
+      <c r="D58" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="B59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="3">
+        <v>42378</v>
+      </c>
+      <c r="D59" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="B60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="3">
+        <v>42378</v>
+      </c>
+      <c r="D60" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="3">
+        <v>42378</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="3">
+        <v>42379</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="3">
+        <v>42381</v>
+      </c>
+      <c r="D63" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="3">
+        <v>42381</v>
+      </c>
+      <c r="D64" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="B65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="3">
+        <v>42382</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="3">
+        <v>42383</v>
+      </c>
+      <c r="D66" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="3">
+        <v>42384</v>
+      </c>
+      <c r="D67" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="B68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="3">
+        <v>42384</v>
+      </c>
+      <c r="D68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="3">
+        <v>42384</v>
+      </c>
+      <c r="D69" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D22">
-    <sortState ref="B3:D47">
+  <autoFilter ref="B2:D69">
+    <sortState ref="B3:D66">
       <sortCondition ref="C2:C22"/>
     </sortState>
   </autoFilter>

</xml_diff>